<commit_message>
Update U1 and U7 silkscreen placement to be ready for next revision, V0.5 assembly BOM reviewed during first assembly
</commit_message>
<xml_diff>
--- a/Electronic Design/Core64 LB v0.5/Core64 LB v0.5 BOM.xlsx
+++ b/Electronic Design/Core64 LB v0.5/Core64 LB v0.5 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/Core64 LB v0.5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89733613-48F9-734B-840C-DE9A1672A589}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC668B0F-985C-E947-9B05-28BEA96078DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="31100" windowHeight="22660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37400" windowHeight="22660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Core64 LB v0.5" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="244">
   <si>
     <t>Source:</t>
   </si>
@@ -132,9 +132,6 @@
     <t>0.01uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C9, C6, C4, C5, C11, </t>
-  </si>
-  <si>
     <t>0.1uF</t>
   </si>
   <si>
@@ -519,9 +516,6 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">R5, R43, R53, R55, R54, R56, R7, R13, R14, R8, R3, R10, R44, R45, R2, R1, R48, R49, </t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -531,9 +525,6 @@
     <t>11-1%</t>
   </si>
   <si>
-    <t xml:space="preserve">R15, R9, R16, </t>
-  </si>
-  <si>
     <t>1K5-1%</t>
   </si>
   <si>
@@ -753,13 +744,25 @@
     <t>HDR100IMP40F-G-V-TH‎</t>
   </si>
   <si>
-    <t>Need more of later when they are in stock</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
     <t>Use for Core Board sockets and Teensy 3.2 sockets. Extras for accessories.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R15, R16, </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> R9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5, R43, R53, R55, R54, R56, R7, R13, R14, R8, R1, R48, R49, </t>
+  </si>
+  <si>
+    <t>R3, R10, R44, R45, R2</t>
+  </si>
+  <si>
+    <t>C9, C6, C4, C5,</t>
+  </si>
+  <si>
+    <t>C11</t>
   </si>
 </sst>
 </file>
@@ -1264,12 +1267,26 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1626,62 +1643,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="179" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="88.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="5.5" customWidth="1"/>
-    <col min="3" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="79.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
@@ -1703,8 +1721,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -1723,15 +1741,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
@@ -1743,35 +1761,35 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>26</v>
+    <row r="9" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>243</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
@@ -1783,15 +1801,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
+    <row r="11" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -1803,15 +1821,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
         <v>35</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
@@ -1823,1202 +1841,1247 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>40</v>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B15">
         <v>6</v>
       </c>
       <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
         <v>47</v>
       </c>
-      <c r="B16">
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" t="s">
+        <v>154</v>
+      </c>
+      <c r="E21" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="C23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" t="s">
+        <v>159</v>
+      </c>
+      <c r="F23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24" s="4">
+        <v>470</v>
+      </c>
+      <c r="D24" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" t="s">
+        <v>159</v>
+      </c>
+      <c r="F24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>164</v>
+      </c>
+      <c r="D26" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" t="s">
+        <v>159</v>
+      </c>
+      <c r="F27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" t="s">
+        <v>158</v>
+      </c>
+      <c r="E28" t="s">
+        <v>159</v>
+      </c>
+      <c r="F28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B29">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" t="s">
+        <v>159</v>
+      </c>
+      <c r="F29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D30" t="s">
+        <v>158</v>
+      </c>
+      <c r="E30" t="s">
+        <v>159</v>
+      </c>
+      <c r="F30" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E31" t="s">
+        <v>159</v>
+      </c>
+      <c r="F31" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>171</v>
+      </c>
+      <c r="D32" t="s">
+        <v>158</v>
+      </c>
+      <c r="E32" t="s">
+        <v>159</v>
+      </c>
+      <c r="F32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
         <v>52</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F33" t="s">
         <v>54</v>
       </c>
-      <c r="F17" t="s">
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
         <v>56</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" t="s">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F34" t="s">
         <v>58</v>
       </c>
-      <c r="F18" t="s">
+    </row>
+    <row r="35" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
         <v>60</v>
       </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D35" t="s">
         <v>61</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E35" t="s">
         <v>62</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F35" t="s">
         <v>63</v>
       </c>
-      <c r="F19" t="s">
+    </row>
+    <row r="36" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
         <v>65</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D36" t="s">
         <v>66</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E36" t="s">
         <v>67</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F36" t="s">
         <v>68</v>
       </c>
-      <c r="F20" t="s">
+    </row>
+    <row r="37" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
         <v>70</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D37" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
         <v>72</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D38" t="s">
         <v>73</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E38" t="s">
         <v>74</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F38" t="s">
         <v>75</v>
       </c>
-      <c r="F22" t="s">
+    </row>
+    <row r="39" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
         <v>77</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D39" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" t="s">
         <v>78</v>
       </c>
-      <c r="D23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F39" t="s">
         <v>79</v>
       </c>
-      <c r="F23" t="s">
+    </row>
+    <row r="40" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
         <v>81</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D40" t="s">
         <v>82</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E40" t="s">
         <v>83</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F40" t="s">
         <v>84</v>
       </c>
-      <c r="F24" t="s">
+    </row>
+    <row r="41" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
         <v>86</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D41" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" t="s">
+        <v>83</v>
+      </c>
+      <c r="F41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D25" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E42" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" t="s">
         <v>83</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F43" t="s">
         <v>84</v>
       </c>
-      <c r="F25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="44" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D27" t="s">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D44" t="s">
+        <v>82</v>
+      </c>
+      <c r="E44" t="s">
         <v>83</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F44" t="s">
         <v>84</v>
       </c>
-      <c r="F27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" t="s">
+    </row>
+    <row r="45" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" t="s">
+        <v>82</v>
+      </c>
+      <c r="E45" t="s">
         <v>83</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F45" t="s">
         <v>84</v>
       </c>
-      <c r="F28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="4">
+    </row>
+    <row r="46" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46">
         <v>2</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>103</v>
-      </c>
-      <c r="D30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="C46" t="s">
         <v>104</v>
       </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D46" t="s">
+        <v>104</v>
+      </c>
+      <c r="E46" t="s">
         <v>105</v>
       </c>
-      <c r="D31" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="F46" t="s">
         <v>106</v>
       </c>
-      <c r="F31" t="s">
+    </row>
+    <row r="47" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" t="s">
-        <v>110</v>
-      </c>
-      <c r="F32" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>112</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" t="s">
-        <v>115</v>
-      </c>
-      <c r="F33" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>118</v>
-      </c>
-      <c r="D34" t="s">
-        <v>119</v>
-      </c>
-      <c r="E34" t="s">
-        <v>120</v>
-      </c>
-      <c r="F34" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>123</v>
-      </c>
-      <c r="D35" t="s">
-        <v>119</v>
-      </c>
-      <c r="E35" t="s">
-        <v>124</v>
-      </c>
-      <c r="F35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>125</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>126</v>
-      </c>
-      <c r="D36" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>127</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>129</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>130</v>
-      </c>
-      <c r="D38" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" t="s">
-        <v>124</v>
-      </c>
-      <c r="F38" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>131</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>132</v>
-      </c>
-      <c r="D39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39" t="s">
-        <v>124</v>
-      </c>
-      <c r="F39" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>133</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D40" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40" t="s">
-        <v>124</v>
-      </c>
-      <c r="F40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>135</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D41" t="s">
-        <v>136</v>
-      </c>
-      <c r="E41" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>138</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>139</v>
-      </c>
-      <c r="D42" t="s">
-        <v>139</v>
-      </c>
-      <c r="E42" t="s">
-        <v>140</v>
-      </c>
-      <c r="F42" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>143</v>
-      </c>
-      <c r="D43" t="s">
-        <v>144</v>
-      </c>
-      <c r="E43" t="s">
-        <v>145</v>
-      </c>
-      <c r="F43" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B44">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>148</v>
-      </c>
-      <c r="D44" t="s">
-        <v>148</v>
-      </c>
-      <c r="E44" t="s">
-        <v>145</v>
-      </c>
-      <c r="F44" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B45">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>151</v>
-      </c>
-      <c r="D45" t="s">
-        <v>151</v>
-      </c>
-      <c r="E45" t="s">
-        <v>145</v>
-      </c>
-      <c r="F45" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>154</v>
-      </c>
-      <c r="D46" t="s">
-        <v>155</v>
-      </c>
-      <c r="E46" t="s">
-        <v>145</v>
-      </c>
-      <c r="F46" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="B47">
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>158</v>
+        <v>104</v>
       </c>
       <c r="D47" t="s">
-        <v>159</v>
+        <v>108</v>
       </c>
       <c r="E47" t="s">
-        <v>160</v>
+        <v>109</v>
       </c>
       <c r="F47" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>162</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="B48">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
       <c r="D48" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="E48" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="F48" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>164</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" t="s">
+        <v>119</v>
+      </c>
+      <c r="F49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E50" t="s">
+        <v>123</v>
+      </c>
+      <c r="F50" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>125</v>
+      </c>
+      <c r="D51" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" t="s">
+        <v>114</v>
+      </c>
+      <c r="F51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>127</v>
+      </c>
+      <c r="D52" t="s">
+        <v>118</v>
+      </c>
+      <c r="E52" t="s">
+        <v>123</v>
+      </c>
+      <c r="F52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" t="s">
+        <v>118</v>
+      </c>
+      <c r="E53" t="s">
+        <v>123</v>
+      </c>
+      <c r="F53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" t="s">
+        <v>123</v>
+      </c>
+      <c r="F54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>133</v>
+      </c>
+      <c r="D55" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" t="s">
+        <v>123</v>
+      </c>
+      <c r="F55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56">
         <v>2</v>
       </c>
-      <c r="C49" t="s">
-        <v>165</v>
-      </c>
-      <c r="D49" t="s">
-        <v>159</v>
-      </c>
-      <c r="E49" t="s">
-        <v>160</v>
-      </c>
-      <c r="F49" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B50">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>167</v>
-      </c>
-      <c r="D50" t="s">
-        <v>159</v>
-      </c>
-      <c r="E50" t="s">
-        <v>160</v>
-      </c>
-      <c r="F50" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B51">
-        <v>6</v>
-      </c>
-      <c r="C51" t="s">
-        <v>169</v>
-      </c>
-      <c r="D51" t="s">
-        <v>159</v>
-      </c>
-      <c r="E51" t="s">
-        <v>160</v>
-      </c>
-      <c r="F51" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B52">
+      <c r="C56" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" t="s">
+        <v>135</v>
+      </c>
+      <c r="E56" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D57" t="s">
+        <v>138</v>
+      </c>
+      <c r="E57" t="s">
+        <v>139</v>
+      </c>
+      <c r="F57" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>180</v>
+      </c>
+      <c r="D58" t="s">
+        <v>180</v>
+      </c>
+      <c r="E58" t="s">
+        <v>181</v>
+      </c>
+      <c r="F58" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>187</v>
+      </c>
+      <c r="D59" t="s">
+        <v>187</v>
+      </c>
+      <c r="E59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F59" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D60" t="s">
+        <v>191</v>
+      </c>
+      <c r="E60" t="s">
+        <v>192</v>
+      </c>
+      <c r="F60" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>195</v>
+      </c>
+      <c r="D61" t="s">
+        <v>195</v>
+      </c>
+      <c r="E61" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>198</v>
+      </c>
+      <c r="D62" t="s">
+        <v>198</v>
+      </c>
+      <c r="E62" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>201</v>
+      </c>
+      <c r="D63" t="s">
+        <v>201</v>
+      </c>
+      <c r="E63" t="s">
+        <v>202</v>
+      </c>
+      <c r="F63" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>205</v>
+      </c>
+      <c r="D64" t="s">
+        <v>205</v>
+      </c>
+      <c r="E64" t="s">
+        <v>206</v>
+      </c>
+      <c r="F64" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>175</v>
+      </c>
+      <c r="D65" t="s">
+        <v>176</v>
+      </c>
+      <c r="E65" t="s">
+        <v>177</v>
+      </c>
+      <c r="F65" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>209</v>
+      </c>
+      <c r="D66" t="s">
+        <v>210</v>
+      </c>
+      <c r="E66" t="s">
+        <v>211</v>
+      </c>
+      <c r="F66" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>214</v>
+      </c>
+      <c r="D67" t="s">
+        <v>215</v>
+      </c>
+      <c r="E67" t="s">
+        <v>216</v>
+      </c>
+      <c r="F67" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>219</v>
+      </c>
+      <c r="D68" t="s">
+        <v>219</v>
+      </c>
+      <c r="E68" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B69" s="3">
+        <v>1</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>225</v>
+      </c>
+      <c r="D70" t="s">
+        <v>226</v>
+      </c>
+      <c r="E70" t="s">
+        <v>227</v>
+      </c>
+      <c r="F70" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B71" s="3">
         <v>2</v>
       </c>
-      <c r="C52" t="s">
-        <v>171</v>
-      </c>
-      <c r="D52" t="s">
-        <v>159</v>
-      </c>
-      <c r="E52" t="s">
-        <v>160</v>
-      </c>
-      <c r="F52" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B53">
-        <v>21</v>
-      </c>
-      <c r="C53">
-        <v>470</v>
-      </c>
-      <c r="D53" t="s">
-        <v>159</v>
-      </c>
-      <c r="E53" t="s">
-        <v>160</v>
-      </c>
-      <c r="F53" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54" t="s">
-        <v>174</v>
-      </c>
-      <c r="D54" t="s">
-        <v>159</v>
-      </c>
-      <c r="E54" t="s">
-        <v>160</v>
-      </c>
-      <c r="F54" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B55">
-        <v>3</v>
-      </c>
-      <c r="C55" t="s">
-        <v>176</v>
-      </c>
-      <c r="D55" t="s">
-        <v>159</v>
-      </c>
-      <c r="E55" t="s">
-        <v>160</v>
-      </c>
-      <c r="F55" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
-        <v>178</v>
-      </c>
-      <c r="D56" t="s">
-        <v>179</v>
-      </c>
-      <c r="E56" t="s">
-        <v>180</v>
-      </c>
-      <c r="F56" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="C71" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="6"/>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>229</v>
+      </c>
+      <c r="D73" t="s">
+        <v>232</v>
+      </c>
+      <c r="E73" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="6"/>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>231</v>
+      </c>
+      <c r="D74" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="D57" t="s">
-        <v>183</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
         <v>184</v>
       </c>
-      <c r="F57" t="s">
+      <c r="D75" t="s">
+        <v>184</v>
+      </c>
+      <c r="E75" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>187</v>
-      </c>
-      <c r="D58" t="s">
-        <v>187</v>
-      </c>
-      <c r="E58" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
-        <v>190</v>
-      </c>
-      <c r="D59" t="s">
-        <v>190</v>
-      </c>
-      <c r="E59" t="s">
-        <v>191</v>
-      </c>
-      <c r="F59" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D60" t="s">
-        <v>194</v>
-      </c>
-      <c r="E60" t="s">
-        <v>195</v>
-      </c>
-      <c r="F60" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>197</v>
-      </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
-        <v>198</v>
-      </c>
-      <c r="D61" t="s">
-        <v>198</v>
-      </c>
-      <c r="E61" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>200</v>
-      </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-      <c r="C62" t="s">
-        <v>201</v>
-      </c>
-      <c r="D62" t="s">
-        <v>201</v>
-      </c>
-      <c r="E62" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63" t="s">
-        <v>204</v>
-      </c>
-      <c r="D63" t="s">
-        <v>204</v>
-      </c>
-      <c r="E63" t="s">
-        <v>205</v>
-      </c>
-      <c r="F63" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>207</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64" t="s">
-        <v>208</v>
-      </c>
-      <c r="D64" t="s">
-        <v>208</v>
-      </c>
-      <c r="E64" t="s">
-        <v>209</v>
-      </c>
-      <c r="F64" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-      <c r="C65" t="s">
-        <v>212</v>
-      </c>
-      <c r="D65" t="s">
-        <v>213</v>
-      </c>
-      <c r="E65" t="s">
-        <v>214</v>
-      </c>
-      <c r="F65" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>216</v>
-      </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66" t="s">
-        <v>217</v>
-      </c>
-      <c r="D66" t="s">
-        <v>218</v>
-      </c>
-      <c r="E66" t="s">
-        <v>219</v>
-      </c>
-      <c r="F66" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" t="s">
-        <v>222</v>
-      </c>
-      <c r="D67" t="s">
-        <v>222</v>
-      </c>
-      <c r="E67" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="B68" s="4">
-        <v>1</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>227</v>
-      </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" t="s">
-        <v>228</v>
-      </c>
-      <c r="D69" t="s">
-        <v>229</v>
-      </c>
-      <c r="E69" t="s">
-        <v>230</v>
-      </c>
-      <c r="F69" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
-      <c r="B71">
-        <v>1</v>
-      </c>
-      <c r="C71" t="s">
-        <v>232</v>
-      </c>
-      <c r="D71" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="6"/>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="6"/>
+      <c r="B79">
+        <v>4</v>
+      </c>
+      <c r="C79" t="s">
         <v>235</v>
       </c>
-      <c r="E71" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72" t="s">
-        <v>234</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="D79" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
-      <c r="B74">
-        <v>1</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="E79" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
-      <c r="B76">
-        <v>4</v>
-      </c>
-      <c r="C76" t="s">
-        <v>238</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E76" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>241</v>
-      </c>
-      <c r="B80">
-        <v>1</v>
-      </c>
-      <c r="C80" t="s">
-        <v>204</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D76" r:id="rId1" display="https://www.digikey.com/product-detail/en/chip-quik-inc/HDR100IMP40F-G-V-TH/HDR100IMP40F-G-V-TH-ND/5978200" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D79" r:id="rId1" display="https://www.digikey.com/product-detail/en/chip-quik-inc/HDR100IMP40F-G-V-TH/HDR100IMP40F-G-V-TH-ND/5978200" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update schematic and BOM hardware ID EEPROM from 128 to 256 Byte
</commit_message>
<xml_diff>
--- a/Electronic Design/Core64 LB v0.5/Core64 LB v0.5 BOM.xlsx
+++ b/Electronic Design/Core64 LB v0.5/Core64 LB v0.5 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/Core64 LB v0.5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC668B0F-985C-E947-9B05-28BEA96078DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A608AC1-9446-3B49-905D-F88D904996BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="37400" windowHeight="22660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -606,15 +606,9 @@
     <t xml:space="preserve">U4, </t>
   </si>
   <si>
-    <t>M24C01-RMN</t>
-  </si>
-  <si>
     <t>Package_SO:SOIC-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
-    <t>1Kb (128x8) I2C Serial EEPROM, 1.8-5.5V, SOIC-8</t>
-  </si>
-  <si>
     <t xml:space="preserve">U5, </t>
   </si>
   <si>
@@ -763,6 +757,12 @@
   </si>
   <si>
     <t>C11</t>
+  </si>
+  <si>
+    <t>M24C02-RMN</t>
+  </si>
+  <si>
+    <t>2Kb (256x8) I2C Serial EEPROM, 1.8-5.5V, SOIC-8</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1269,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1287,6 +1286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1646,12 +1646,12 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="88.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="88.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="5.5" customWidth="1"/>
     <col min="3" max="3" width="30.5" customWidth="1"/>
     <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
@@ -1659,7 +1659,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1667,7 +1667,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -1675,7 +1675,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -1683,7 +1683,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
@@ -1691,7 +1691,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5">
@@ -1699,7 +1699,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
@@ -1722,7 +1722,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B7">
@@ -1742,8 +1742,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>242</v>
+      <c r="A8" s="5" t="s">
+        <v>240</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -1762,8 +1762,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>243</v>
+      <c r="A9" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1782,7 +1782,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B10">
@@ -1802,7 +1802,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B11">
@@ -1822,7 +1822,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B12">
@@ -1842,7 +1842,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B13">
@@ -1862,7 +1862,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B14">
@@ -1882,7 +1882,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B15">
@@ -1902,7 +1902,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B16">
@@ -1922,7 +1922,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B17">
@@ -1942,7 +1942,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>149</v>
       </c>
       <c r="B18">
@@ -1962,7 +1962,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>146</v>
       </c>
       <c r="B19">
@@ -1982,7 +1982,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>141</v>
       </c>
       <c r="B20">
@@ -2002,7 +2002,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>152</v>
       </c>
       <c r="B21">
@@ -2022,7 +2022,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>165</v>
       </c>
       <c r="B22">
@@ -2042,7 +2042,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>162</v>
       </c>
       <c r="B23">
@@ -2062,13 +2062,13 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>169</v>
       </c>
       <c r="B24">
         <v>21</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>470</v>
       </c>
       <c r="D24" t="s">
@@ -2082,8 +2082,8 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>238</v>
+      <c r="A25" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2102,8 +2102,8 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>239</v>
+      <c r="A26" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2122,7 +2122,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>156</v>
       </c>
       <c r="B27">
@@ -2142,7 +2142,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>167</v>
       </c>
       <c r="B28">
@@ -2162,8 +2162,8 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>240</v>
+      <c r="A29" s="5" t="s">
+        <v>238</v>
       </c>
       <c r="B29">
         <v>13</v>
@@ -2182,8 +2182,8 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>241</v>
+      <c r="A30" s="7" t="s">
+        <v>239</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -2202,7 +2202,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>172</v>
       </c>
       <c r="B31">
@@ -2222,7 +2222,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>170</v>
       </c>
       <c r="B32">
@@ -2242,7 +2242,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B33">
@@ -2262,7 +2262,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B34">
@@ -2282,7 +2282,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B35">
@@ -2302,7 +2302,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>64</v>
       </c>
       <c r="B36">
@@ -2322,7 +2322,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B37">
@@ -2342,7 +2342,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B38">
@@ -2362,7 +2362,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B39">
@@ -2382,7 +2382,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B40">
@@ -2402,7 +2402,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B41">
@@ -2422,7 +2422,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B42">
@@ -2442,7 +2442,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>92</v>
       </c>
       <c r="B43">
@@ -2462,7 +2462,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B44">
@@ -2482,7 +2482,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B45">
@@ -2502,7 +2502,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B46">
@@ -2522,7 +2522,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B47">
@@ -2542,7 +2542,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B48">
@@ -2562,7 +2562,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="4" t="s">
         <v>116</v>
       </c>
       <c r="B49">
@@ -2582,7 +2582,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B50">
@@ -2602,7 +2602,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="4" t="s">
         <v>124</v>
       </c>
       <c r="B51">
@@ -2622,7 +2622,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>126</v>
       </c>
       <c r="B52">
@@ -2642,7 +2642,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B53">
@@ -2662,7 +2662,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B54">
@@ -2682,7 +2682,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>132</v>
       </c>
       <c r="B55">
@@ -2702,7 +2702,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B56">
@@ -2719,7 +2719,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>137</v>
       </c>
       <c r="B57">
@@ -2739,7 +2739,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="5" t="s">
         <v>179</v>
       </c>
       <c r="B58">
@@ -2759,7 +2759,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>186</v>
       </c>
       <c r="B59">
@@ -2779,101 +2779,101 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="5" t="s">
         <v>190</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="D60" t="s">
+        <v>242</v>
+      </c>
+      <c r="E60" t="s">
         <v>191</v>
       </c>
-      <c r="D60" t="s">
-        <v>191</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="F60" t="s">
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
+      <c r="D61" t="s">
+        <v>193</v>
+      </c>
+      <c r="E61" t="s">
         <v>194</v>
       </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
+    </row>
+    <row r="62" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D61" t="s">
-        <v>195</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
+      <c r="D62" t="s">
+        <v>196</v>
+      </c>
+      <c r="E62" t="s">
         <v>197</v>
       </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-      <c r="C62" t="s">
+    </row>
+    <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="D62" t="s">
-        <v>198</v>
-      </c>
-      <c r="E62" t="s">
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
+      <c r="D63" t="s">
+        <v>199</v>
+      </c>
+      <c r="E63" t="s">
         <v>200</v>
       </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="F63" t="s">
         <v>201</v>
       </c>
-      <c r="D63" t="s">
-        <v>201</v>
-      </c>
-      <c r="E63" t="s">
+    </row>
+    <row r="64" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="F63" t="s">
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
+      <c r="D64" t="s">
+        <v>203</v>
+      </c>
+      <c r="E64" t="s">
         <v>204</v>
       </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="F64" t="s">
         <v>205</v>
       </c>
-      <c r="D64" t="s">
-        <v>205</v>
-      </c>
-      <c r="E64" t="s">
-        <v>206</v>
-      </c>
-      <c r="F64" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="5" t="s">
         <v>174</v>
       </c>
       <c r="B65">
@@ -2893,151 +2893,151 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>207</v>
+      </c>
+      <c r="D66" t="s">
         <v>208</v>
       </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="E66" t="s">
         <v>209</v>
       </c>
-      <c r="D66" t="s">
+      <c r="F66" t="s">
         <v>210</v>
       </c>
-      <c r="E66" t="s">
+    </row>
+    <row r="67" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F66" t="s">
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
+      <c r="D67" t="s">
         <v>213</v>
       </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="E67" t="s">
         <v>214</v>
       </c>
-      <c r="D67" t="s">
+      <c r="F67" t="s">
         <v>215</v>
       </c>
-      <c r="E67" t="s">
+    </row>
+    <row r="68" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="F67" t="s">
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
+      <c r="D68" t="s">
+        <v>217</v>
+      </c>
+      <c r="E68" t="s">
         <v>218</v>
       </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68" t="s">
+    </row>
+    <row r="69" spans="1:6" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D68" t="s">
-        <v>219</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="B69" s="2">
+        <v>1</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="7" t="s">
+      <c r="D69" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B69" s="3">
-        <v>1</v>
-      </c>
-      <c r="C69" s="3" t="s">
+      <c r="F69" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E69" s="3" t="s">
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
         <v>223</v>
       </c>
-      <c r="F69" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
+      <c r="D70" t="s">
         <v>224</v>
       </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="E70" t="s">
         <v>225</v>
       </c>
-      <c r="D70" t="s">
+      <c r="F70" t="s">
         <v>226</v>
       </c>
-      <c r="E70" t="s">
+    </row>
+    <row r="71" spans="1:6" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B71" s="2">
+        <v>2</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="5"/>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
         <v>227</v>
       </c>
-      <c r="F70" t="s">
+      <c r="D73" t="s">
+        <v>230</v>
+      </c>
+      <c r="E73" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B71" s="3">
-        <v>2</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="6"/>
-      <c r="B73">
-        <v>1</v>
-      </c>
-      <c r="C73" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="5"/>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
         <v>229</v>
       </c>
-      <c r="D73" t="s">
-        <v>232</v>
-      </c>
-      <c r="E73" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="6"/>
-      <c r="B74">
-        <v>1</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>231</v>
       </c>
-      <c r="D74" t="s">
-        <v>233</v>
-      </c>
     </row>
     <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="5" t="s">
         <v>183</v>
       </c>
       <c r="B75">
@@ -3054,27 +3054,27 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="6"/>
+      <c r="A77" s="5"/>
       <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="6"/>
+      <c r="A79" s="5"/>
       <c r="B79">
         <v>4</v>
       </c>
       <c r="C79" t="s">
+        <v>233</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E79" t="s">
         <v>235</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E79" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update connectors on BOM
</commit_message>
<xml_diff>
--- a/Electronic Design/Core64 LB v0.5/Core64 LB v0.5 BOM.xlsx
+++ b/Electronic Design/Core64 LB v0.5/Core64 LB v0.5 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Electronic Design/Core64 LB v0.5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A608AC1-9446-3B49-905D-F88D904996BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AEABC5-40BD-DF4D-9D70-99862D70890C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="37400" windowHeight="22660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20760" yWindow="460" windowWidth="32940" windowHeight="22660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Core64 LB v0.5" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="244">
   <si>
     <t>Source:</t>
   </si>
@@ -735,12 +735,6 @@
     <t>40p Socket in LB from CB</t>
   </si>
   <si>
-    <t>HDR100IMP40F-G-V-TH‎</t>
-  </si>
-  <si>
-    <t>Use for Core Board sockets and Teensy 3.2 sockets. Extras for accessories.</t>
-  </si>
-  <si>
     <t xml:space="preserve">R15, R16, </t>
   </si>
   <si>
@@ -763,6 +757,12 @@
   </si>
   <si>
     <t>2Kb (256x8) I2C Serial EEPROM, 1.8-5.5V, SOIC-8</t>
+  </si>
+  <si>
+    <t>Use for Core Board sockets. Extras for accessories.</t>
+  </si>
+  <si>
+    <t>HDR100IMP40F-G-V-TH</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1267,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1287,6 +1287,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1643,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1743,7 +1744,7 @@
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -1763,7 +1764,7 @@
     </row>
     <row r="9" spans="1:7" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -2083,7 +2084,7 @@
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2103,7 +2104,7 @@
     </row>
     <row r="26" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2163,7 +2164,7 @@
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B29">
         <v>13</v>
@@ -2183,7 +2184,7 @@
     </row>
     <row r="30" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -2786,16 +2787,16 @@
         <v>1</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D60" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E60" t="s">
         <v>191</v>
       </c>
       <c r="F60" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -2932,40 +2933,23 @@
         <v>215</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68" t="s">
-        <v>217</v>
-      </c>
-      <c r="D68" t="s">
-        <v>217</v>
-      </c>
-      <c r="E68" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
+    <row r="69" spans="1:6" s="9" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B69" s="2">
-        <v>1</v>
-      </c>
-      <c r="C69" s="2" t="s">
+      <c r="B69" s="9">
+        <v>1</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D69" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E69" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F69" s="9" t="s">
         <v>210</v>
       </c>
     </row>
@@ -2989,26 +2973,6 @@
         <v>226</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B71" s="2">
-        <v>2</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="5"/>
       <c r="B73">
@@ -3062,19 +3026,58 @@
         <v>232</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="5"/>
+    <row r="78" spans="1:6" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B78" s="2">
+        <v>1</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="B79">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C79" t="s">
         <v>233</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="E79" t="s">
-        <v>235</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>